<commit_message>
arquivo e imagem de exemplo do excel.
</commit_message>
<xml_diff>
--- a/uploads/modelo.xlsx
+++ b/uploads/modelo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win10\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan\OneDrive\Área de Trabalho\sistemas\Financeiro\financial-api\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FBE0FFC5-F763-4170-A243-755197CAB418}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{BCC2F48B-E6EF-4C16-8906-3D7240DA6A27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Tipo</t>
   </si>
@@ -40,9 +39,6 @@
   </si>
   <si>
     <t>Numero do Documento</t>
-  </si>
-  <si>
-    <t>Mês de Competencia</t>
   </si>
   <si>
     <t>Débito / Crédito</t>
@@ -60,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,11 +407,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676BB981-BA7B-4F6F-90D2-E37459CEA21D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,29 +440,25 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>